<commit_message>
Added census FIPS code + land cover data
</commit_message>
<xml_diff>
--- a/data/raw_data/mpdata_ALL.xlsx
+++ b/data/raw_data/mpdata_ALL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ameliafoley/Desktop/MADA/AmeliaFoley-MADA-project/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C280BF-E971-5044-99FC-22AB6F0947C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE94B31-34DC-454C-AE2F-0EFF1D9EF308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="500" windowWidth="23580" windowHeight="16560" xr2:uid="{ACB3E58D-9E99-BC4E-9343-6DFFD2F0CC0E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="81">
   <si>
     <t>volume_ml</t>
   </si>
@@ -655,7 +655,7 @@
   <dimension ref="A1:K93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2676,9 +2676,15 @@
       <c r="A61" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+      <c r="B61" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="2">
+        <v>33.955800000000004</v>
+      </c>
+      <c r="D61" s="2">
+        <v>-83.400499999999994</v>
+      </c>
       <c r="E61" s="2">
         <v>150</v>
       </c>
@@ -3710,9 +3716,15 @@
       <c r="A92" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
+      <c r="B92" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C92" s="2">
+        <v>33.955800000000004</v>
+      </c>
+      <c r="D92" s="2">
+        <v>-83.400499999999994</v>
+      </c>
       <c r="E92" s="2">
         <v>150</v>
       </c>

</xml_diff>